<commit_message>
Updated BSBM results to include 0.8.1 results
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM v3 Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM v3 Benchmark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="330" windowWidth="24675" windowHeight="10515" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="30">
   <si>
     <t>Test Data</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Dataset Size in Triples vs QMpH</t>
+  </si>
+  <si>
+    <t>Leviathan 0.8.1</t>
   </si>
 </sst>
 </file>
@@ -195,15 +198,9 @@
   </cellStyleXfs>
   <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,9 +222,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -235,6 +229,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -257,7 +260,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -492,6 +495,103 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'In-Memory Comparisons'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leviathan 0.8.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>725515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900517</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.0030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3289999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0339999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9960000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1660000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1929999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2060000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -500,11 +600,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="86614016"/>
-        <c:axId val="78593408"/>
+        <c:axId val="100319808"/>
+        <c:axId val="100320384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="86614016"/>
+        <c:axId val="100319808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,12 +637,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78593408"/>
+        <c:crossAx val="100320384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="78593408"/>
+        <c:axId val="100320384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -577,7 +677,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86614016"/>
+        <c:crossAx val="100319808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -602,7 +702,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -648,7 +748,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$8</c:f>
+              <c:f>'In-Memory Comparisons'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -662,7 +762,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$7:$K$7</c:f>
+              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -701,7 +801,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
+              <c:f>'In-Memory Comparisons'!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -745,7 +845,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'In-Memory Comparisons'!$A$9</c:f>
+              <c:f>'In-Memory Comparisons'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -759,7 +859,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$7:$K$7</c:f>
+              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="10"/>
@@ -798,7 +898,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'In-Memory Comparisons'!$B$9:$K$9</c:f>
+              <c:f>'In-Memory Comparisons'!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -831,6 +931,103 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>6679.68</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'In-Memory Comparisons'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leviathan 0.8.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$8:$K$8</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>725515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900517</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$11:$K$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25702.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24558.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25817.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25588.799999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25730.69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25662.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25117.74</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>25024.71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25097.41</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24978.46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,11 +1042,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="97214848"/>
-        <c:axId val="97200768"/>
+        <c:axId val="58766400"/>
+        <c:axId val="58766976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="97214848"/>
+        <c:axId val="58766400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -878,12 +1075,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97200768"/>
+        <c:crossAx val="58766976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="97200768"/>
+        <c:axId val="58766976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -920,7 +1117,352 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97214848"/>
+        <c:crossAx val="58766400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Leviathan Parellel vs Non-Parallel In-Memory Performance</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> on BSBM v3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'In-Memory Comparisons'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leviathan 0.6.0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>725515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900517</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$4:$K$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.933999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17.372</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.843</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.623000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.558</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.253</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>26.946999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'In-Memory Comparisons'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Leviathan 0.8.1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$2:$K$2</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4991</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98113</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>191502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>375114</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>550078</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>725515</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900517</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000313</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'In-Memory Comparisons'!$B$5:$K$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>7.0030000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3289999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9720000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0339999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9960000000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.1660000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.1929999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.1719999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2060000000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="46714240"/>
+        <c:axId val="100322688"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="46714240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dataset Size</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Triples</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="100322688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="100322688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Total Runtime</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> in Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="46714240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -948,14 +1490,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -978,13 +1520,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>104776</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -999,6 +1541,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>52388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6" title="Leviathan BSBM v3 Performance"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1294,10 +1868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17:I26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,806 +1888,1172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="C2" s="3"/>
+      <c r="A2" s="1"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="5">
         <v>10</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="6">
         <v>4991</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="5">
         <v>10</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E6" s="5">
         <v>50</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <v>0.19750000000000001</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="10">
         <v>0.59950000000000003</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <v>12.911</v>
       </c>
-      <c r="I6" s="12">
+      <c r="I6" s="10">
         <v>13942.09</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="10">
         <v>0.25821</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="10">
         <v>0.25258999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="5">
         <v>50</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="6">
         <v>22716</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="5">
         <v>10</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
         <v>50</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <v>0.21629999999999999</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="10">
         <v>0.40450000000000003</v>
       </c>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <v>13.083</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="10">
         <v>13785.19</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="10">
         <v>0.26166</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="10">
         <v>0.25997999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="5">
         <v>100</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="6">
         <v>40333</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="5">
         <v>10</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="5">
         <v>50</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>0.25569999999999998</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>0.53239999999999998</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>16.241</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <v>11082.87</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="10">
         <v>0.32483000000000001</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="10">
         <v>0.32089000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>250</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="6">
         <v>98113</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="5">
         <v>10</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="5">
         <v>50</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>0.31119999999999998</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="10">
         <v>0.74729999999999996</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <v>27.239000000000001</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="10">
         <v>6608.18</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="10">
         <v>0.54478000000000004</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="10">
         <v>0.53708999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>500</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="6">
         <v>191502</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="5">
         <v>50</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="10">
         <v>0.30059999999999998</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="10">
         <v>1.1022000000000001</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <v>38.332000000000001</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="10">
         <v>4695.79</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="10">
         <v>0.76663999999999999</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="10">
         <v>0.74114999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="5">
         <v>1000</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="6">
         <v>375114</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="5">
         <v>50</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>0.26119999999999999</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <v>2.3521000000000001</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>54.933999999999997</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="10">
         <v>3276.64</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J11" s="10">
         <v>1.0986899999999999</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="10">
         <v>0.99868999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="8">
         <v>1500</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="9">
         <v>550078</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="5">
         <v>10</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
         <v>50</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="10">
         <v>0.3997</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="10">
         <v>7.5995999999999997</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <v>125.60299999999999</v>
       </c>
-      <c r="I12" s="12">
+      <c r="I12" s="10">
         <v>1433.08</v>
       </c>
-      <c r="J12" s="12">
+      <c r="J12" s="10">
         <v>2.51207</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="10">
         <v>2.16133</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="8">
         <v>2000</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="9">
         <v>725515</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="5">
         <v>10</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="5">
         <v>50</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>0.755</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="10">
         <v>8.0890000000000004</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <v>204.999</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="10">
         <v>878.05</v>
       </c>
-      <c r="J13" s="12">
+      <c r="J13" s="10">
         <v>4.0999800000000004</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="10">
         <v>3.5819200000000002</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="8">
         <v>2500</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="9">
         <v>900517</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="5">
         <v>50</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>1.31</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="10">
         <v>17.051100000000002</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <v>302.77600000000001</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <v>594.5</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="10">
         <v>6.0555199999999996</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="10">
         <v>5.2458799999999997</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="14">
+      <c r="A15" s="11">
         <v>2785</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="9">
         <v>1000313</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>10</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>50</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="10">
         <v>1.53</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="10">
         <v>14.383800000000001</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <v>370.24099999999999</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="10">
         <v>486.17</v>
       </c>
-      <c r="J15" s="12">
+      <c r="J15" s="10">
         <v>7.40482</v>
       </c>
-      <c r="K15" s="12">
+      <c r="K15" s="10">
         <v>6.5285500000000001</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
+      <c r="A17" s="5">
         <v>10</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="6">
         <v>4991</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="5">
         <v>10</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
         <v>50</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="10">
         <v>0.17299999999999999</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="10">
         <v>0.23519999999999999</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H17" s="10">
         <v>9.6150000000000002</v>
       </c>
-      <c r="I17" s="12">
+      <c r="I17" s="10">
         <v>18721.009999999998</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="10">
         <v>0.1923</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="10">
         <v>0.19173999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="7">
+      <c r="A18" s="5">
         <v>50</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="6">
         <v>22716</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="5">
         <v>10</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="5">
         <v>50</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="10">
         <v>0.1787</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G18" s="10">
         <v>0.26869999999999999</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <v>10.14</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="10">
         <v>17751.37</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="10">
         <v>0.20280000000000001</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="10">
         <v>0.2021</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="5">
         <v>100</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="6">
         <v>40333</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="5">
         <v>10</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="5">
         <v>50</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="10">
         <v>0.19040000000000001</v>
       </c>
-      <c r="G19" s="12">
+      <c r="G19" s="10">
         <v>0.25030000000000002</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H19" s="10">
         <v>10.933999999999999</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="10">
         <v>16463.080000000002</v>
       </c>
-      <c r="J19" s="12">
+      <c r="J19" s="10">
         <v>0.21867</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="10">
         <v>0.21823999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="5">
         <v>250</v>
       </c>
-      <c r="B20" s="8">
+      <c r="B20" s="6">
         <v>98113</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="5">
         <v>10</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="5">
         <v>50</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <v>0.20569999999999999</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="10">
         <v>0.89380000000000004</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H20" s="10">
         <v>14.315</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="10">
         <v>12573.83</v>
       </c>
-      <c r="J20" s="12">
+      <c r="J20" s="10">
         <v>0.28631000000000001</v>
       </c>
-      <c r="K20" s="12">
+      <c r="K20" s="10">
         <v>0.27937000000000001</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="5">
         <v>500</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="6">
         <v>191502</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="5">
         <v>10</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="5">
         <v>50</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F21" s="10">
         <v>0.24060000000000001</v>
       </c>
-      <c r="G21" s="12">
+      <c r="G21" s="10">
         <v>0.72609999999999997</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="10">
         <v>17.372</v>
       </c>
-      <c r="I21" s="12">
+      <c r="I21" s="10">
         <v>10361.57</v>
       </c>
-      <c r="J21" s="12">
+      <c r="J21" s="10">
         <v>0.34744000000000003</v>
       </c>
-      <c r="K21" s="12">
+      <c r="K21" s="10">
         <v>0.34117999999999998</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="5">
         <v>1000</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="6">
         <v>375114</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="5">
         <v>10</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
         <v>50</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="10">
         <v>0.21820000000000001</v>
       </c>
-      <c r="G22" s="12">
+      <c r="G22" s="10">
         <v>0.4778</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="10">
         <v>15.843</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="10">
         <v>11361.44</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="10">
         <v>0.31685999999999998</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="10">
         <v>0.31319000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
+      <c r="A23" s="8">
         <v>1500</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="9">
         <v>550078</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="5">
         <v>10</v>
       </c>
-      <c r="E23" s="7">
+      <c r="E23" s="5">
         <v>50</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="10">
         <v>0.25779999999999997</v>
       </c>
-      <c r="G23" s="12">
+      <c r="G23" s="10">
         <v>0.59240000000000004</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="10">
         <v>19.623000000000001</v>
       </c>
-      <c r="I23" s="12">
+      <c r="I23" s="10">
         <v>9172.9500000000007</v>
       </c>
-      <c r="J23" s="12">
+      <c r="J23" s="10">
         <v>0.39245999999999998</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="10">
         <v>0.38673000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
+      <c r="A24" s="8">
         <v>2000</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="9">
         <v>725515</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="7">
+      <c r="D24" s="5">
         <v>10</v>
       </c>
-      <c r="E24" s="7">
+      <c r="E24" s="5">
         <v>50</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <v>0.26619999999999999</v>
       </c>
-      <c r="G24" s="12">
+      <c r="G24" s="10">
         <v>0.84689999999999999</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H24" s="10">
         <v>22.558</v>
       </c>
-      <c r="I24" s="12">
+      <c r="I24" s="10">
         <v>7979.48</v>
       </c>
-      <c r="J24" s="12">
+      <c r="J24" s="10">
         <v>0.45116000000000001</v>
       </c>
-      <c r="K24" s="12">
+      <c r="K24" s="10">
         <v>0.44183</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="8">
         <v>2500</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="9">
         <v>900517</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="5">
         <v>10</v>
       </c>
-      <c r="E25" s="7">
+      <c r="E25" s="5">
         <v>50</v>
       </c>
-      <c r="F25" s="12">
+      <c r="F25" s="10">
         <v>0.3387</v>
       </c>
-      <c r="G25" s="12">
+      <c r="G25" s="10">
         <v>0.83750000000000002</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H25" s="10">
         <v>26.253</v>
       </c>
-      <c r="I25" s="12">
+      <c r="I25" s="10">
         <v>6856.41</v>
       </c>
-      <c r="J25" s="12">
+      <c r="J25" s="10">
         <v>0.52505999999999997</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="10">
         <v>0.51507000000000003</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="14">
+      <c r="A26" s="11">
         <v>2785</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="9">
         <v>1000313</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="16">
+      <c r="D26" s="13">
         <v>10</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="13">
         <v>50</v>
       </c>
-      <c r="F26" s="12">
+      <c r="F26" s="10">
         <v>0.3508</v>
       </c>
-      <c r="G26" s="12">
+      <c r="G26" s="10">
         <v>0.71679999999999999</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H26" s="10">
         <v>26.946999999999999</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="10">
         <v>6679.68</v>
       </c>
-      <c r="J26" s="12">
+      <c r="J26" s="10">
         <v>0.53895000000000004</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="10">
         <v>0.53037000000000001</v>
       </c>
     </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>10</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4991</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="5">
+        <v>10</v>
+      </c>
+      <c r="E28" s="5">
+        <v>50</v>
+      </c>
+      <c r="F28" s="10">
+        <v>0.13089999999999999</v>
+      </c>
+      <c r="G28" s="10">
+        <v>0.20019999999999999</v>
+      </c>
+      <c r="H28" s="10">
+        <v>7.0030000000000001</v>
+      </c>
+      <c r="I28" s="10">
+        <v>25702.85</v>
+      </c>
+      <c r="J28" s="10">
+        <v>0.14005999999999999</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0.13971</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>50</v>
+      </c>
+      <c r="B29" s="6">
+        <v>22716</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="5">
+        <v>10</v>
+      </c>
+      <c r="E29" s="5">
+        <v>50</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.1305</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.1822</v>
+      </c>
+      <c r="H29" s="10">
+        <v>7.3289999999999997</v>
+      </c>
+      <c r="I29" s="10">
+        <v>24558.92</v>
+      </c>
+      <c r="J29" s="10">
+        <v>0.14659</v>
+      </c>
+      <c r="K29" s="10">
+        <v>0.14616000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>100</v>
+      </c>
+      <c r="B30" s="6">
+        <v>40333</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="5">
+        <v>10</v>
+      </c>
+      <c r="E30" s="5">
+        <v>50</v>
+      </c>
+      <c r="F30" s="10">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G30" s="10">
+        <v>0.15559999999999999</v>
+      </c>
+      <c r="H30" s="10">
+        <v>6.9720000000000004</v>
+      </c>
+      <c r="I30" s="10">
+        <v>25817.48</v>
+      </c>
+      <c r="J30" s="10">
+        <v>0.13944000000000001</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0.13932</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>250</v>
+      </c>
+      <c r="B31" s="6">
+        <v>98113</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="5">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5">
+        <v>50</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0.12820000000000001</v>
+      </c>
+      <c r="G31" s="10">
+        <v>0.20569999999999999</v>
+      </c>
+      <c r="H31" s="10">
+        <v>7.0339999999999998</v>
+      </c>
+      <c r="I31" s="10">
+        <v>25588.799999999999</v>
+      </c>
+      <c r="J31" s="10">
+        <v>0.14069000000000001</v>
+      </c>
+      <c r="K31" s="10">
+        <v>0.14027999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>500</v>
+      </c>
+      <c r="B32" s="6">
+        <v>191502</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="5">
+        <v>10</v>
+      </c>
+      <c r="E32" s="5">
+        <v>50</v>
+      </c>
+      <c r="F32" s="10">
+        <v>0.13089999999999999</v>
+      </c>
+      <c r="G32" s="10">
+        <v>0.15110000000000001</v>
+      </c>
+      <c r="H32" s="10">
+        <v>6.9960000000000004</v>
+      </c>
+      <c r="I32" s="10">
+        <v>25730.69</v>
+      </c>
+      <c r="J32" s="10">
+        <v>0.13991000000000001</v>
+      </c>
+      <c r="K32" s="10">
+        <v>0.13980999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>1000</v>
+      </c>
+      <c r="B33" s="6">
+        <v>375114</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="5">
+        <v>10</v>
+      </c>
+      <c r="E33" s="5">
+        <v>50</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0.12590000000000001</v>
+      </c>
+      <c r="G33" s="10">
+        <v>0.2024</v>
+      </c>
+      <c r="H33" s="10">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="I33" s="10">
+        <v>25662.14</v>
+      </c>
+      <c r="J33" s="10">
+        <v>0.14027999999999999</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0.13991000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>1500</v>
+      </c>
+      <c r="B34" s="9">
+        <v>550078</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="5">
+        <v>10</v>
+      </c>
+      <c r="E34" s="5">
+        <v>50</v>
+      </c>
+      <c r="F34" s="10">
+        <v>0.1333</v>
+      </c>
+      <c r="G34" s="10">
+        <v>0.1736</v>
+      </c>
+      <c r="H34" s="10">
+        <v>7.1660000000000004</v>
+      </c>
+      <c r="I34" s="10">
+        <v>25117.74</v>
+      </c>
+      <c r="J34" s="10">
+        <v>0.14332</v>
+      </c>
+      <c r="K34" s="10">
+        <v>0.1431</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>2000</v>
+      </c>
+      <c r="B35" s="9">
+        <v>725515</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="5">
+        <v>10</v>
+      </c>
+      <c r="E35" s="5">
+        <v>50</v>
+      </c>
+      <c r="F35" s="10">
+        <v>0.1298</v>
+      </c>
+      <c r="G35" s="10">
+        <v>0.26879999999999998</v>
+      </c>
+      <c r="H35" s="10">
+        <v>7.1929999999999996</v>
+      </c>
+      <c r="I35" s="10">
+        <v>25024.71</v>
+      </c>
+      <c r="J35" s="10">
+        <v>0.14385999999999999</v>
+      </c>
+      <c r="K35" s="10">
+        <v>0.1429</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>2500</v>
+      </c>
+      <c r="B36" s="9">
+        <v>900517</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="5">
+        <v>10</v>
+      </c>
+      <c r="E36" s="5">
+        <v>50</v>
+      </c>
+      <c r="F36" s="10">
+        <v>0.1265</v>
+      </c>
+      <c r="G36" s="10">
+        <v>0.29649999999999999</v>
+      </c>
+      <c r="H36" s="10">
+        <v>7.1719999999999997</v>
+      </c>
+      <c r="I36" s="10">
+        <v>25097.41</v>
+      </c>
+      <c r="J36" s="10">
+        <v>0.14344000000000001</v>
+      </c>
+      <c r="K36" s="10">
+        <v>0.14201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>2785</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1000313</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="13">
+        <v>10</v>
+      </c>
+      <c r="E37" s="13">
+        <v>50</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.13270000000000001</v>
+      </c>
+      <c r="G37" s="10">
+        <v>0.16259999999999999</v>
+      </c>
+      <c r="H37" s="10">
+        <v>7.2060000000000004</v>
+      </c>
+      <c r="I37" s="10">
+        <v>24978.46</v>
+      </c>
+      <c r="J37" s="10">
+        <v>0.14412</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0.14399999999999999</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A16:K16"/>
+    <mergeCell ref="A27:K27"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:K3"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="179" orientation="portrait" r:id="rId1"/>
@@ -2122,10 +3062,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R14"/>
+  <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,235 +3089,305 @@
       <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8">
+      <c r="A2" s="10"/>
+      <c r="B2" s="6">
         <v>4991</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="6">
         <v>22716</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="6">
         <v>40333</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="6">
         <v>98113</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="6">
         <v>191502</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="6">
         <v>375114</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>550078</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="9">
         <v>725515</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="9">
         <v>900517</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="9">
         <v>1000313</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="10">
         <v>12.911</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="10">
         <v>13.083</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="10">
         <v>16.241</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="10">
         <v>27.239000000000001</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <v>38.332000000000001</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <v>54.933999999999997</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <v>125.60299999999999</v>
       </c>
-      <c r="I3" s="12">
+      <c r="I3" s="10">
         <v>204.999</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="10">
         <v>302.77600000000001</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="10">
         <v>370.24099999999999</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>9.6150000000000002</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="10">
         <v>10.14</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="10">
         <v>10.933999999999999</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="10">
         <v>14.315</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <v>17.372</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <v>15.843</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <v>19.623000000000001</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="10">
         <v>22.558</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="10">
         <v>26.253</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="10">
         <v>26.946999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="10">
+        <v>7.0030000000000001</v>
+      </c>
+      <c r="C5" s="10">
+        <v>7.3289999999999997</v>
+      </c>
+      <c r="D5" s="10">
+        <v>6.9720000000000004</v>
+      </c>
+      <c r="E5" s="10">
+        <v>7.0339999999999998</v>
+      </c>
+      <c r="F5" s="10">
+        <v>6.9960000000000004</v>
+      </c>
+      <c r="G5" s="10">
+        <v>7.0140000000000002</v>
+      </c>
+      <c r="H5" s="10">
+        <v>7.1660000000000004</v>
+      </c>
+      <c r="I5" s="10">
+        <v>7.1929999999999996</v>
+      </c>
+      <c r="J5" s="10">
+        <v>7.1719999999999997</v>
+      </c>
+      <c r="K5" s="10">
+        <v>7.2060000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="8">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="6">
         <v>4991</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C8" s="6">
         <v>22716</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D8" s="6">
         <v>40333</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E8" s="6">
         <v>98113</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="6">
         <v>191502</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G8" s="6">
         <v>375114</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H8" s="9">
         <v>550078</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I8" s="9">
         <v>725515</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J8" s="9">
         <v>900517</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K8" s="9">
         <v>1000313</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B9" s="10">
         <v>13942.09</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C9" s="10">
         <v>13785.19</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D9" s="10">
         <v>11082.87</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E9" s="10">
         <v>6608.18</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F9" s="10">
         <v>4695.79</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G9" s="10">
         <v>3276.64</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H9" s="10">
         <v>1433.08</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I9" s="10">
         <v>878.05</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J9" s="10">
         <v>594.5</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K9" s="10">
         <v>486.17</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B10" s="10">
         <v>18721.009999999998</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C10" s="10">
         <v>17751.37</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D10" s="10">
         <v>16463.080000000002</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E10" s="10">
         <v>12573.83</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F10" s="10">
         <v>10361.57</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G10" s="10">
         <v>11361.44</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H10" s="10">
         <v>9172.9500000000007</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I10" s="10">
         <v>7979.48</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J10" s="10">
         <v>6856.41</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K10" s="10">
         <v>6679.68</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="R14" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="10">
+        <v>25702.85</v>
+      </c>
+      <c r="C11" s="10">
+        <v>24558.92</v>
+      </c>
+      <c r="D11" s="10">
+        <v>25817.48</v>
+      </c>
+      <c r="E11" s="10">
+        <v>25588.799999999999</v>
+      </c>
+      <c r="F11" s="10">
+        <v>25730.69</v>
+      </c>
+      <c r="G11" s="10">
+        <v>25662.14</v>
+      </c>
+      <c r="H11" s="10">
+        <v>25117.74</v>
+      </c>
+      <c r="I11" s="10">
+        <v>25024.71</v>
+      </c>
+      <c r="J11" s="10">
+        <v>25097.41</v>
+      </c>
+      <c r="K11" s="10">
+        <v>24978.46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R15" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A6:K6"/>
+    <mergeCell ref="A7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>